<commit_message>
Added boards with SPI flash and SD
There are sub-folders holding a board using SPI flash, and one with both SD and SPI flash.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>WM3983CT-ND</t>
   </si>
@@ -59,12 +59,6 @@
     <t>MicroSD Socket</t>
   </si>
   <si>
-    <t>1660</t>
-  </si>
-  <si>
-    <t>Adafruit</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -96,6 +90,18 @@
   </si>
   <si>
     <t>1k Res</t>
+  </si>
+  <si>
+    <t>Cost per board</t>
+  </si>
+  <si>
+    <t>Cost per part</t>
+  </si>
+  <si>
+    <t>WM12834CT-ND</t>
+  </si>
+  <si>
+    <t>Total cost of parts:</t>
   </si>
 </sst>
 </file>
@@ -129,6 +135,7 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -144,7 +151,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -194,6 +201,111 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -207,12 +319,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -227,6 +336,19 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -544,10 +666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,162 +677,236 @@
     <col min="1" max="2" width="16.85546875" customWidth="1"/>
     <col min="3" max="3" width="21.85546875" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="C2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="8">
+        <v>1</v>
+      </c>
+      <c r="E2" s="14">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F2" s="18">
+        <f>PRODUCT(D2,E2)</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="8">
+        <v>1</v>
+      </c>
+      <c r="E3" s="15">
+        <v>0.6</v>
+      </c>
+      <c r="F3" s="19">
+        <f t="shared" ref="F3:F10" si="0">PRODUCT(D3,E3)</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="8">
+        <v>8</v>
+      </c>
+      <c r="E4" s="15">
+        <v>0.02</v>
+      </c>
+      <c r="F4" s="19">
+        <f t="shared" si="0"/>
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="8">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="9">
+      <c r="E5" s="15">
+        <v>6.95</v>
+      </c>
+      <c r="F5" s="19">
+        <f t="shared" si="0"/>
+        <v>13.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="8">
+        <v>4</v>
+      </c>
+      <c r="E6" s="15">
+        <v>0.24</v>
+      </c>
+      <c r="F6" s="19">
+        <f t="shared" si="0"/>
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="9">
         <v>1</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="10">
-        <v>1</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="1"/>
+      <c r="E7" s="16">
+        <v>2.12</v>
+      </c>
+      <c r="F7" s="19">
+        <f t="shared" si="0"/>
+        <v>2.12</v>
+      </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="8">
+        <v>2</v>
+      </c>
+      <c r="E8" s="15">
+        <v>0.02</v>
+      </c>
+      <c r="F8" s="19">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="D9" s="8">
+        <v>1</v>
+      </c>
+      <c r="E9" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F9" s="19">
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="5" t="s">
+      <c r="B10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D10" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="9">
-        <v>1</v>
+      <c r="E10" s="17">
+        <v>0.01</v>
+      </c>
+      <c r="F10" s="20">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E11" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="13">
+        <f>SUM(F2:F10)</f>
+        <v>19.990000000000002</v>
       </c>
     </row>
   </sheetData>
@@ -723,8 +919,9 @@
     <hyperlink ref="C8" r:id="rId6" display="https://www.digikey.com/product-detail/en/kemet/C0805C106K8PACTU/399-4925-2-ND/1090830"/>
     <hyperlink ref="C9" r:id="rId7" display="https://www.digikey.com/product-detail/en/cts-electrocomponents/204-211ST/CT204211ST-ND/267310"/>
     <hyperlink ref="C10" r:id="rId8" display="https://www.digikey.com/product-detail/en/samsung-electro-mechanics/RC1608J912CS/1276-5085-2-ND/3965392"/>
+    <hyperlink ref="C7" r:id="rId9" display="https://www.digikey.com/product-detail/en/molex-llc/5031821852/WM12834CT-ND/5823232"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId9"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>